<commit_message>
ingreso validaciones 3 y 4 ok
</commit_message>
<xml_diff>
--- a/integrantesfamiliareceptora.xlsx
+++ b/integrantesfamiliareceptora.xlsx
@@ -38,9 +38,6 @@
     <t>ApellidoMaterno</t>
   </si>
   <si>
-    <t xml:space="preserve">Sexo </t>
-  </si>
-  <si>
     <t>Edad</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>19.114.777-0</t>
+  </si>
+  <si>
+    <t>Sexo</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,13 +445,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -459,117 +459,117 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>